<commit_message>
Fix extracol key computation.
</commit_message>
<xml_diff>
--- a/test_data/bom_merge.xlsx
+++ b/test_data/bom_merge.xlsx
@@ -45,7 +45,7 @@
     <t xml:space="preserve">MountTechnology</t>
   </si>
   <si>
-    <t xml:space="preserve">NODE 123</t>
+    <t xml:space="preserve">NODE acquisto</t>
   </si>
   <si>
     <t xml:space="preserve">CODE farnell</t>
@@ -126,7 +126,7 @@
     <t xml:space="preserve">due</t>
   </si>
   <si>
-    <t xml:space="preserve">J3, j4</t>
+    <t xml:space="preserve">J3, J4</t>
   </si>
   <si>
     <t xml:space="preserve">C10</t>
@@ -262,8 +262,8 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>